<commit_message>
more work on type data
more formatting work on the type lookup table
</commit_message>
<xml_diff>
--- a/Pokemon_type_excel.xlsx
+++ b/Pokemon_type_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Zackry Finer\Documents\GitHub\Pokemon-Battle-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298379FE-0507-4E68-B7C9-AC2B1336A465}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A498E46C-1512-408F-ADC8-6C389F61C3B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2EEA683-B595-4BD1-B911-76B049F5F409}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>×</t>
   </si>
@@ -70,6 +70,60 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>"normal":0</t>
+  </si>
+  <si>
+    <t>"flight":1</t>
+  </si>
+  <si>
+    <t>"flying":2</t>
+  </si>
+  <si>
+    <t>"poison":3</t>
+  </si>
+  <si>
+    <t>"ground":4</t>
+  </si>
+  <si>
+    <t>"rock":5</t>
+  </si>
+  <si>
+    <t>"bug":6</t>
+  </si>
+  <si>
+    <t>"ghost":7</t>
+  </si>
+  <si>
+    <t>"steel":8</t>
+  </si>
+  <si>
+    <t>"fire":9</t>
+  </si>
+  <si>
+    <t>"water":10</t>
+  </si>
+  <si>
+    <t>"grass":11</t>
+  </si>
+  <si>
+    <t>"electric":12</t>
+  </si>
+  <si>
+    <t>"psychic":13</t>
+  </si>
+  <si>
+    <t>"ice":14</t>
+  </si>
+  <si>
+    <t>"dragon":15</t>
+  </si>
+  <si>
+    <t>"dark":16</t>
+  </si>
+  <si>
+    <t>"fairy":17</t>
   </si>
 </sst>
 </file>
@@ -3099,10 +3153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B87D813-66F4-43A5-B5BA-7618EA6C7B5B}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,6 +4280,62 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>27</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" t="s">
+        <v>29</v>
+      </c>
+      <c r="T22" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B2"/>

</xml_diff>